<commit_message>
missed in last commit
</commit_message>
<xml_diff>
--- a/clients/DiveInsurance/data/template/Phly_Group.xlsx
+++ b/clients/DiveInsurance/data/template/Phly_Group.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Cert_No</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>{{certificate_type}}</t>
+  </si>
+  <si>
+    <t>{{renewal}}</t>
   </si>
   <si>
     <t>{{group_cvrg_level}}</t>
@@ -198,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -207,9 +210,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,33 +562,35 @@
       <c r="O2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="3"/>
+      <c r="P2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="Q2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>